<commit_message>
Added 0198 - DK:ERST
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$80</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="372">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1198,6 +1198,28 @@
   </si>
   <si>
     <t>Also called "Numéro d'identification suisse des enterprises (IDE)"</t>
+  </si>
+  <si>
+    <t>Norwegian VAT number</t>
+  </si>
+  <si>
+    <t>0198</t>
+  </si>
+  <si>
+    <t>ERSTORG</t>
+  </si>
+  <si>
+    <t>DK:ERST</t>
+  </si>
+  <si>
+    <t>The Danish Business Authority</t>
+  </si>
+  <si>
+    <t>DKXXXXXXXX
+Two characters (DK) followed by 8 digits eg. DK12345678</t>
+  </si>
+  <si>
+    <t>10 characters, no space or other separator</t>
   </si>
 </sst>
 </file>
@@ -1597,11 +1619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK79"/>
+  <dimension ref="A1:AMK80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2271,78 +2293,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="72.5">
+    <row r="23" spans="1:11" ht="29">
       <c r="A23" s="1" t="s">
-        <v>136</v>
+        <v>368</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>366</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>139</v>
+        <v>367</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>140</v>
+        <v>369</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="2">
-        <f>0</f>
+      <c r="G23" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="72.5">
+      <c r="A24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="29">
-      <c r="A24" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
@@ -2351,25 +2373,28 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>149</v>
+      <c r="I25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>17</v>
@@ -2379,24 +2404,24 @@
         <v>0</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="29">
       <c r="A27" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
@@ -2411,16 +2436,19 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>17</v>
@@ -2430,24 +2458,21 @@
         <v>0</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="87">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>
@@ -2457,24 +2482,24 @@
         <v>0</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="29">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="87">
       <c r="A30" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
@@ -2483,13 +2508,16 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K30" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="29">
       <c r="A31" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>115</v>
@@ -2497,112 +2525,114 @@
       <c r="D31" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E31"/>
+      <c r="E31" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="29">
+      <c r="A32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K32" s="3">
         <v>990399123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33"/>
+        <v>174</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G33" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:12">
+      <c r="A35" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="43.5">
-      <c r="A35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>17</v>
@@ -2611,24 +2641,20 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="36" spans="1:12" ht="29">
       <c r="A36" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36"/>
+        <v>186</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>17</v>
       </c>
@@ -2636,49 +2662,44 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K36" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="29">
       <c r="A37" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>195</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E37"/>
       <c r="F37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G37" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="29">
       <c r="A38" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>133</v>
+        <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>17</v>
@@ -2688,71 +2709,72 @@
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="43.5">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:12" ht="43.5">
+      <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E39"/>
-      <c r="F39" s="1" t="s">
+      <c r="E40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G39" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="1" t="s">
+      <c r="G40" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="E40"/>
-      <c r="F40" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G40" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="29">
-      <c r="A41" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E41"/>
       <c r="F41" s="1" t="s">
@@ -2762,43 +2784,50 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="I41" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="29">
       <c r="A42" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E42"/>
-      <c r="F42" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G42" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E43"/>
+      <c r="E43" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="F43" s="1" t="s">
         <v>170</v>
       </c>
@@ -2809,16 +2838,16 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E44"/>
       <c r="F44" s="1" t="s">
@@ -2831,16 +2860,16 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E45"/>
       <c r="F45" s="1" t="s">
@@ -2853,16 +2882,16 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>121</v>
+        <v>223</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E46"/>
       <c r="F46" s="1" t="s">
@@ -2875,16 +2904,16 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>230</v>
+        <v>121</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E47"/>
       <c r="F47" s="1" t="s">
@@ -2897,16 +2926,16 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E48"/>
       <c r="F48" s="1" t="s">
@@ -2919,17 +2948,18 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>239</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="E49"/>
       <c r="F49" s="1" t="s">
         <v>170</v>
       </c>
@@ -2940,18 +2970,17 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E50"/>
+        <v>239</v>
+      </c>
       <c r="F50" s="1" t="s">
         <v>170</v>
       </c>
@@ -2962,16 +2991,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E51"/>
       <c r="F51" s="1" t="s">
@@ -2984,16 +3013,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>109</v>
+        <v>246</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E52"/>
       <c r="F52" s="1" t="s">
@@ -3005,17 +3034,17 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="9" t="s">
-        <v>251</v>
+      <c r="A53" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E53"/>
       <c r="F53" s="1" t="s">
@@ -3028,16 +3057,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E54"/>
       <c r="F54" s="1" t="s">
@@ -3050,16 +3079,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="1" t="s">
@@ -3072,16 +3101,16 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="9" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="1" t="s">
@@ -3094,16 +3123,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="1" t="s">
@@ -3116,16 +3145,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>138</v>
+        <v>269</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="1" t="s">
@@ -3138,16 +3167,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>276</v>
+        <v>138</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="1" t="s">
@@ -3160,16 +3189,16 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="1" t="s">
@@ -3182,16 +3211,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="1" t="s">
@@ -3204,16 +3233,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="1" t="s">
@@ -3224,18 +3253,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="29">
+    <row r="63" spans="1:7">
       <c r="A63" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="1" t="s">
@@ -3246,18 +3275,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" ht="29">
       <c r="A64" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="1" t="s">
@@ -3270,16 +3299,16 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>69</v>
+        <v>296</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="1" t="s">
@@ -3292,16 +3321,16 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>303</v>
+        <v>69</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="1" t="s">
@@ -3314,16 +3343,16 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="1" t="s">
@@ -3336,16 +3365,16 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="9" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="1" t="s">
@@ -3358,16 +3387,16 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="1" t="s">
@@ -3380,16 +3409,16 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E70"/>
       <c r="F70" s="1" t="s">
@@ -3402,16 +3431,16 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="1" t="s">
@@ -3424,17 +3453,18 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>328</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="E72"/>
       <c r="F72" s="1" t="s">
         <v>170</v>
       </c>
@@ -3445,18 +3475,17 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E73"/>
+        <v>328</v>
+      </c>
       <c r="F73" s="1" t="s">
         <v>170</v>
       </c>
@@ -3467,16 +3496,16 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E74"/>
       <c r="F74" s="1" t="s">
@@ -3488,92 +3517,90 @@
       </c>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E75"/>
+      <c r="F75" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G75" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G76" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:12">
+      <c r="A77" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G76" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="29">
-      <c r="A77" s="1" t="s">
+      <c r="G77" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="29">
+      <c r="A78" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G77" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>100</v>
@@ -3582,33 +3609,57 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" ht="43.5">
+      <c r="I78" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G79" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="43.5">
+      <c r="A80" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G79" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="L79" s="1" t="s">
+      <c r="G80" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>357</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L78"/>
+  <autoFilter ref="A1:L80"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added 0199 - LEI
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$81</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="378">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1220,6 +1220,32 @@
   </si>
   <si>
     <t>10 characters, no space or other separator</t>
+  </si>
+  <si>
+    <t>0199</t>
+  </si>
+  <si>
+    <t>Legal Entity Identifier (LEI)</t>
+  </si>
+  <si>
+    <t>As of December 2018, there are 33 LEI issuing organizations in the world.</t>
+  </si>
+  <si>
+    <t>The entire 20 character code (including the check digits)</t>
+  </si>
+  <si>
+    <t>The ISO 17442 standard specifies the minimum reference data, which must the format of the organization identifiers, be Supplied for each LEI:
+* The official name of the legal entity as recorded in the official registers.
+* The registered address of that legal entity.
+* The country of formation.
+* The codes for the representation of names of countries and their subdivisions.
+* The date of the first LEI assignment; the date of last update of the
+* LEI information; and the date of expiry, if applicable.
+Additional information may be registered as agreed between the legal entity and its LEI issuing organization.
+etc. - see ICD sheet for further information</t>
+  </si>
+  <si>
+    <t>LEI</t>
   </si>
 </sst>
 </file>
@@ -1619,11 +1645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK80"/>
+  <dimension ref="A1:AMK81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:D23"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2323,78 +2349,78 @@
         <v>371</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="72.5">
+    <row r="24" spans="1:11" ht="174">
       <c r="A24" s="1" t="s">
-        <v>136</v>
+        <v>377</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>372</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>139</v>
+        <v>373</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>140</v>
+        <v>374</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="2">
-        <f>0</f>
+      <c r="G24" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="72.5">
+      <c r="A25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="29">
-      <c r="A25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>17</v>
@@ -2403,25 +2429,28 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>149</v>
+      <c r="I26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29">
       <c r="A27" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
@@ -2431,24 +2460,24 @@
         <v>0</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="29">
       <c r="A28" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>17</v>
@@ -2463,16 +2492,19 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>
@@ -2482,24 +2514,21 @@
         <v>0</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="87">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
@@ -2509,24 +2538,24 @@
         <v>0</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="29">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="87">
       <c r="A31" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>
@@ -2535,125 +2564,131 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K31" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="29">
       <c r="A32" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>365</v>
+        <v>167</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G32" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="29">
+      <c r="A33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K33" s="3">
         <v>990399123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34"/>
+        <v>174</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G34" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:12">
+      <c r="A36" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="29">
-      <c r="A36" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>17</v>
@@ -2662,24 +2697,20 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="37" spans="1:12" ht="29">
       <c r="A37" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E37"/>
+        <v>186</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>17</v>
       </c>
@@ -2687,43 +2718,44 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K37" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="29">
       <c r="A38" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E38"/>
       <c r="F38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G38" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="29">
       <c r="A39" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>133</v>
+        <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>17</v>
@@ -2733,77 +2765,74 @@
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="43.5">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:12" ht="43.5">
+      <c r="A41" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G40" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="1" t="s">
+      <c r="G41" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E41"/>
-      <c r="F41" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G41" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="29">
-      <c r="A42" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>195</v>
-      </c>
+      <c r="E42"/>
       <c r="F42" s="1" t="s">
         <v>196</v>
       </c>
@@ -2811,45 +2840,50 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="I42" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="29">
       <c r="A43" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G43" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E44"/>
       <c r="F44" s="1" t="s">
         <v>170</v>
       </c>
@@ -2860,16 +2894,16 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E45"/>
       <c r="F45" s="1" t="s">
@@ -2882,16 +2916,16 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E46"/>
       <c r="F46" s="1" t="s">
@@ -2904,16 +2938,16 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>121</v>
+        <v>223</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E47"/>
       <c r="F47" s="1" t="s">
@@ -2926,16 +2960,16 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>230</v>
+        <v>121</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E48"/>
       <c r="F48" s="1" t="s">
@@ -2948,16 +2982,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E49"/>
       <c r="F49" s="1" t="s">
@@ -2970,17 +3004,18 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>239</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="E50"/>
       <c r="F50" s="1" t="s">
         <v>170</v>
       </c>
@@ -2991,18 +3026,17 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E51"/>
+        <v>239</v>
+      </c>
       <c r="F51" s="1" t="s">
         <v>170</v>
       </c>
@@ -3013,16 +3047,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E52"/>
       <c r="F52" s="1" t="s">
@@ -3035,16 +3069,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>246</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E53"/>
       <c r="F53" s="1" t="s">
@@ -3056,17 +3090,17 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="9" t="s">
-        <v>251</v>
+      <c r="A54" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E54"/>
       <c r="F54" s="1" t="s">
@@ -3079,16 +3113,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="1" t="s">
@@ -3101,16 +3135,16 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="1" t="s">
@@ -3123,16 +3157,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="1" t="s">
@@ -3145,16 +3179,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="1" t="s">
@@ -3167,16 +3201,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>138</v>
+        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="1" t="s">
@@ -3189,16 +3223,16 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>276</v>
+        <v>138</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="1" t="s">
@@ -3211,16 +3245,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="1" t="s">
@@ -3233,16 +3267,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="1" t="s">
@@ -3255,16 +3289,16 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="1" t="s">
@@ -3275,18 +3309,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29">
+    <row r="64" spans="1:7">
       <c r="A64" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="1" t="s">
@@ -3297,18 +3331,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" ht="29">
       <c r="A65" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="1" t="s">
@@ -3321,16 +3355,16 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>69</v>
+        <v>296</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="1" t="s">
@@ -3343,16 +3377,16 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>303</v>
+        <v>69</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="1" t="s">
@@ -3365,16 +3399,16 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="1" t="s">
@@ -3387,16 +3421,16 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="9" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="1" t="s">
@@ -3409,16 +3443,16 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E70"/>
       <c r="F70" s="1" t="s">
@@ -3431,16 +3465,16 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="1" t="s">
@@ -3453,16 +3487,16 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E72"/>
       <c r="F72" s="1" t="s">
@@ -3475,17 +3509,18 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>328</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="E73"/>
       <c r="F73" s="1" t="s">
         <v>170</v>
       </c>
@@ -3496,18 +3531,17 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E74"/>
+        <v>328</v>
+      </c>
       <c r="F74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3518,16 +3552,16 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E75"/>
       <c r="F75" s="1" t="s">
@@ -3539,92 +3573,90 @@
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E76"/>
+      <c r="F76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G76" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G77" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H77" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="L77" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:12">
+      <c r="A78" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G77" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="29">
-      <c r="A78" s="1" t="s">
+      <c r="G78" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="29">
+      <c r="A79" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G78" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>100</v>
@@ -3633,33 +3665,57 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="43.5">
+      <c r="I79" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G80" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="43.5">
+      <c r="A81" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G80" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="L80" s="1" t="s">
+      <c r="G81" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L81" s="1" t="s">
         <v>357</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L80"/>
+  <autoFilter ref="A1:L81"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>